<commit_message>
vishakhasayre: vlookup and documentadd for v and h lookup
</commit_message>
<xml_diff>
--- a/Day 12.xlsx
+++ b/Day 12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data analytics\Excel\Day 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F04E0DD-7475-48A5-9673-0C7BF2F04ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB5C938-07A9-4453-9913-C8279E6A014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D83D4149-0CD8-4660-B09D-755CE1F530DD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>shop_name</t>
   </si>
@@ -777,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB6EE39-7555-4889-BDCE-33B41651A53A}">
-  <dimension ref="C4:I15"/>
+  <dimension ref="B4:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,7 +789,7 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
@@ -812,30 +812,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="D5" s="7" t="str">
+        <f>HLOOKUP(D4,$C$13:$I$15,2,FALSE)</f>
+        <v>automotive sq, near tp road , 400001</v>
+      </c>
+      <c r="E5" s="7" t="str">
+        <f t="shared" ref="E5:I5" si="0">HLOOKUP(E4,$C$13:$I$15,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -858,7 +864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -881,30 +887,36 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
+      <c r="D8" s="2" t="str">
+        <f>HLOOKUP(D4,$C$13:$I$15,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f t="shared" ref="E8:I8" si="1">HLOOKUP(E4,$C$13:$I$15,3,FALSE)</f>
+        <v>online</v>
       </c>
       <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G8" s="2">
+        <f t="shared" si="1"/>
         <v>15000</v>
       </c>
       <c r="H8" s="2">
+        <f t="shared" si="1"/>
         <v>2000000</v>
       </c>
       <c r="I8" s="2">
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
@@ -927,7 +939,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -950,7 +962,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="C13" s="6" t="s">
         <v>0</v>
       </c>
@@ -973,7 +988,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>2</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1014,10 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>3</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>